<commit_message>
change 'naive' to correct form
</commit_message>
<xml_diff>
--- a/prep_data.xlsx
+++ b/prep_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hongjiadong/Desktop/mcm23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\mcm23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51616251-B743-AA46-AAE0-03FE1D704B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A7B05A-E286-42F6-90CF-3C743F1C85EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1039,9 +1039,6 @@
     <t>knock</t>
   </si>
   <si>
-    <t>naïve</t>
-  </si>
-  <si>
     <t>apply</t>
   </si>
   <si>
@@ -1132,6 +1129,10 @@
   </si>
   <si>
     <t>Contest_num</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>naive</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1142,7 +1143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,7 +1210,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1225,7 +1226,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1547,53 +1548,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P354"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="D335" sqref="D335"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
     <col min="15" max="15" width="22" customWidth="1"/>
     <col min="16" max="16" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>3</v>
@@ -1605,7 +1606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>358</v>
       </c>
@@ -1655,7 +1656,7 @@
         <v>1.689197569142999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>357</v>
       </c>
@@ -1705,7 +1706,7 @@
         <v>1.7368944760253389E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>356</v>
       </c>
@@ -1755,7 +1756,7 @@
         <v>2.0912360484056099E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>355</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>2.092706330389979E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>354</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>1.960618663893943E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>352</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>2.520229646037702E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>351</v>
       </c>
@@ -1955,7 +1956,7 @@
         <v>2.3512543956951688E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>350</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>2.2610258402953179E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>349</v>
       </c>
@@ -2055,7 +2056,7 @@
         <v>2.363925213134932E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>348</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>2.538288095698862E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>347</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>2.80878026702874E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>346</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>2.5279557554290111E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>345</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>2.7008083159810459E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>344</v>
       </c>
@@ -2305,7 +2306,7 @@
         <v>2.7067114314627352E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>343</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>2.8365681252562228E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>342</v>
       </c>
@@ -2405,7 +2406,7 @@
         <v>2.8266692352433419E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>341</v>
       </c>
@@ -2455,7 +2456,7 @@
         <v>3.2231686805819303E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>340</v>
       </c>
@@ -2505,7 +2506,7 @@
         <v>3.1504609195235962E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>339</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>3.3613584346514611E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>338</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>3.4507178071624019E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>337</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>3.7539398184316147E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>336</v>
       </c>
@@ -2705,7 +2706,7 @@
         <v>3.7009130962262937E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>335</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>3.9105898801100832E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>334</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>3.9104753980205909E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>333</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>3.8690450800908827E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>332</v>
       </c>
@@ -2905,7 +2906,7 @@
         <v>3.9250306707782089E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>331</v>
       </c>
@@ -2955,7 +2956,7 @@
         <v>4.0787210756722952E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>330</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>4.1183944572799627E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>329</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>4.287796608048846E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>328</v>
       </c>
@@ -3105,7 +3106,7 @@
         <v>4.4100341459336757E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>327</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>4.6282803891363779E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>326</v>
       </c>
@@ -3205,7 +3206,7 @@
         <v>4.5708966321274337E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>325</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>4.5341419645547068E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>324</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>4.422136928779976E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>323</v>
       </c>
@@ -3355,7 +3356,7 @@
         <v>3.8127721231162093E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>322</v>
       </c>
@@ -3405,7 +3406,7 @@
         <v>3.4496174296459597E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>320</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>3.9549405210289039E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>319</v>
       </c>
@@ -3505,7 +3506,7 @@
         <v>3.5933656665601242E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>318</v>
       </c>
@@ -3555,7 +3556,7 @@
         <v>3.7070146796400673E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>317</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>3.7330081899866377E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>316</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>3.853143214773147E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>315</v>
       </c>
@@ -3705,7 +3706,7 @@
         <v>3.9815533052099158E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>314</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>4.0591864064455217E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>313</v>
       </c>
@@ -3805,7 +3806,7 @@
         <v>3.9059164570858639E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>312</v>
       </c>
@@ -3855,7 +3856,7 @@
         <v>3.856297901787463E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>311</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>4.1109461913133701E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>310</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>4.1508094178095853E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>309</v>
       </c>
@@ -4005,7 +4006,7 @@
         <v>4.5668934417581387E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>308</v>
       </c>
@@ -4055,7 +4056,7 @@
         <v>4.0613940079641503E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>307</v>
       </c>
@@ -4105,7 +4106,7 @@
         <v>4.1683139453622613E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>306</v>
       </c>
@@ -4155,7 +4156,7 @@
         <v>4.1900642787163371E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>305</v>
       </c>
@@ -4205,7 +4206,7 @@
         <v>4.4045690584957747E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>304</v>
       </c>
@@ -4255,7 +4256,7 @@
         <v>4.2024220377452362E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>303</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>4.3600896599421707E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>302</v>
       </c>
@@ -4355,7 +4356,7 @@
         <v>4.6119864526579298E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>301</v>
       </c>
@@ -4405,7 +4406,7 @@
         <v>4.5259792513973773E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>300</v>
       </c>
@@ -4455,7 +4456,7 @@
         <v>4.533955488460395E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>299</v>
       </c>
@@ -4505,7 +4506,7 @@
         <v>4.493698392003477E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>298</v>
       </c>
@@ -4555,7 +4556,7 @@
         <v>4.7076005070539301E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>297</v>
       </c>
@@ -4605,7 +4606,7 @@
         <v>4.6754443778214957E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>296</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>4.7681967024760151E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>295</v>
       </c>
@@ -4705,7 +4706,7 @@
         <v>5.4782658637767337E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>294</v>
       </c>
@@ -4755,7 +4756,7 @@
         <v>4.8701112736853618E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>293</v>
       </c>
@@ -4805,7 +4806,7 @@
         <v>4.9806058984819102E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>292</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>5.0553919506380593E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>291</v>
       </c>
@@ -4905,7 +4906,7 @@
         <v>4.94146064923221E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>290</v>
       </c>
@@ -4955,7 +4956,7 @@
         <v>5.1566172150411281E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>289</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>5.2327128839363343E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>288</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>5.1737752321637097E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>287</v>
       </c>
@@ -5105,7 +5106,7 @@
         <v>5.4474733064211731E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>286</v>
       </c>
@@ -5155,7 +5156,7 @@
         <v>5.4307780652570858E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>285</v>
       </c>
@@ -5205,7 +5206,7 @@
         <v>5.2984404155820217E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>284</v>
       </c>
@@ -5255,7 +5256,7 @@
         <v>5.4988417904483611E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>283</v>
       </c>
@@ -5305,7 +5306,7 @@
         <v>5.4565168861817143E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>282</v>
       </c>
@@ -5355,7 +5356,7 @@
         <v>5.5114570641051422E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>281</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>5.7005133258320739E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>280</v>
       </c>
@@ -5455,7 +5456,7 @@
         <v>6.2712782679071877E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>279</v>
       </c>
@@ -5505,7 +5506,7 @@
         <v>6.0041820775013903E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>278</v>
       </c>
@@ -5555,7 +5556,7 @@
         <v>6.1101004053058218E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>277</v>
       </c>
@@ -5605,7 +5606,7 @@
         <v>5.6979942308982359E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>276</v>
       </c>
@@ -5655,7 +5656,7 @@
         <v>5.8922846356686209E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>275</v>
       </c>
@@ -5705,7 +5706,7 @@
         <v>6.2631730747897851E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>274</v>
       </c>
@@ -5755,7 +5756,7 @@
         <v>6.1618549858967968E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>273</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>6.0066159828216593E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>272</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>6.3686442038993998E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>271</v>
       </c>
@@ -5905,7 +5906,7 @@
         <v>6.1264471542834223E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>270</v>
       </c>
@@ -5955,7 +5956,7 @@
         <v>6.3466165661359972E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>269</v>
       </c>
@@ -6005,7 +6006,7 @@
         <v>6.4146076568015201E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>268</v>
       </c>
@@ -6055,7 +6056,7 @@
         <v>6.4325201042790062E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>267</v>
       </c>
@@ -6105,7 +6106,7 @@
         <v>6.3829184318281648E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>266</v>
       </c>
@@ -6155,7 +6156,7 @@
         <v>6.3609269055957082E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>265</v>
       </c>
@@ -6205,7 +6206,7 @@
         <v>6.2531190342281828E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>264</v>
       </c>
@@ -6255,7 +6256,7 @@
         <v>6.5884838110500055E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>263</v>
       </c>
@@ -6305,7 +6306,7 @@
         <v>6.3312069760763048E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>262</v>
       </c>
@@ -6355,7 +6356,7 @@
         <v>6.3567400916798508E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>261</v>
       </c>
@@ -6405,7 +6406,7 @@
         <v>6.4840279246879629E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>260</v>
       </c>
@@ -6455,7 +6456,7 @@
         <v>6.5558384811256171E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>259</v>
       </c>
@@ -6505,7 +6506,7 @@
         <v>6.5146730624982635E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>258</v>
       </c>
@@ -6555,7 +6556,7 @@
         <v>6.5691172748661902E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>257</v>
       </c>
@@ -6605,7 +6606,7 @@
         <v>6.5321267451482881E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>256</v>
       </c>
@@ -6655,7 +6656,7 @@
         <v>7.5280764745314463E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>255</v>
       </c>
@@ -6705,7 +6706,7 @@
         <v>6.6622878822041626E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>254</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>7.1053034556684186E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>253</v>
       </c>
@@ -6805,7 +6806,7 @@
         <v>6.4839975845410625E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>252</v>
       </c>
@@ -6855,7 +6856,7 @@
         <v>6.7830309118687343E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>251</v>
       </c>
@@ -6905,7 +6906,7 @@
         <v>6.9193038624143166E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>250</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>7.1536243282212614E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>249</v>
       </c>
@@ -7005,7 +7006,7 @@
         <v>6.6212325380745105E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>248</v>
       </c>
@@ -7055,7 +7056,7 @@
         <v>6.632513868259117E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>247</v>
       </c>
@@ -7105,7 +7106,7 @@
         <v>7.0975790680423492E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>245</v>
       </c>
@@ -7155,7 +7156,7 @@
         <v>7.3713633624392552E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>244</v>
       </c>
@@ -7205,7 +7206,7 @@
         <v>7.3385871384789719E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>243</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>6.8274729985466784E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>242</v>
       </c>
@@ -7305,7 +7306,7 @@
         <v>6.9228707598727526E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>241</v>
       </c>
@@ -7355,7 +7356,7 @@
         <v>6.7220417633410676E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>240</v>
       </c>
@@ -7405,7 +7406,7 @@
         <v>7.3424906081717631E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>239</v>
       </c>
@@ -7455,7 +7456,7 @@
         <v>7.1855502542861632E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>238</v>
       </c>
@@ -7505,7 +7506,7 @@
         <v>7.0281232372612745E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>237</v>
       </c>
@@ -7555,7 +7556,7 @@
         <v>7.2478557047905345E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>236</v>
       </c>
@@ -7605,7 +7606,7 @@
         <v>6.9108982143660319E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>235</v>
       </c>
@@ -7655,7 +7656,7 @@
         <v>7.3764984142342629E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>234</v>
       </c>
@@ -7705,7 +7706,7 @@
         <v>7.1595800921380556E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>233</v>
       </c>
@@ -7755,7 +7756,7 @@
         <v>7.1610746237099093E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>232</v>
       </c>
@@ -7805,7 +7806,7 @@
         <v>7.1173551588580269E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>231</v>
       </c>
@@ -7855,7 +7856,7 @@
         <v>7.224308637760328E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>230</v>
       </c>
@@ -7905,7 +7906,7 @@
         <v>7.3947701706026964E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>229</v>
       </c>
@@ -7955,7 +7956,7 @@
         <v>7.5772871585538928E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>228</v>
       </c>
@@ -8005,7 +8006,7 @@
         <v>7.2707219818444052E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>227</v>
       </c>
@@ -8055,7 +8056,7 @@
         <v>7.4986812384185683E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>226</v>
       </c>
@@ -8105,7 +8106,7 @@
         <v>7.2786238014664412E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>225</v>
       </c>
@@ -8155,7 +8156,7 @@
         <v>7.4952778890733221E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>224</v>
       </c>
@@ -8205,7 +8206,7 @@
         <v>7.4430508576046939E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>223</v>
       </c>
@@ -8255,7 +8256,7 @@
         <v>7.2567700893843234E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>222</v>
       </c>
@@ -8305,7 +8306,7 @@
         <v>7.3851063509506099E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>221</v>
       </c>
@@ -8355,7 +8356,7 @@
         <v>7.5875670558535821E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>220</v>
       </c>
@@ -8405,7 +8406,7 @@
         <v>7.708496085965276E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>219</v>
       </c>
@@ -8455,7 +8456,7 @@
         <v>7.4903462682787872E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>218</v>
       </c>
@@ -8505,7 +8506,7 @@
         <v>7.5838736960811948E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>217</v>
       </c>
@@ -8555,7 +8556,7 @@
         <v>7.5945995438578967E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>216</v>
       </c>
@@ -8605,7 +8606,7 @@
         <v>7.8027410756698751E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>215</v>
       </c>
@@ -8655,7 +8656,7 @@
         <v>7.7760829273893287E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>214</v>
       </c>
@@ -8705,7 +8706,7 @@
         <v>7.6503951057863881E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>213</v>
       </c>
@@ -8755,7 +8756,7 @@
         <v>7.5852690501415215E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>212</v>
       </c>
@@ -8805,7 +8806,7 @@
         <v>7.7841966121609707E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>211</v>
       </c>
@@ -8855,7 +8856,7 @@
         <v>7.5759196711039103E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>210</v>
       </c>
@@ -8905,7 +8906,7 @@
         <v>7.6068860168546082E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>209</v>
       </c>
@@ -8955,7 +8956,7 @@
         <v>7.6298071838979173E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>208</v>
       </c>
@@ -9005,7 +9006,7 @@
         <v>7.7772837648346388E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>207</v>
       </c>
@@ -9055,7 +9056,7 @@
         <v>7.5265718499432116E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>206</v>
       </c>
@@ -9105,7 +9106,7 @@
         <v>7.5492413069839087E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>205</v>
       </c>
@@ -9155,7 +9156,7 @@
         <v>7.7724091969343559E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>204</v>
       </c>
@@ -9205,7 +9206,7 @@
         <v>7.8084368679572372E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>203</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>7.8659686670002699E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>202</v>
       </c>
@@ -9305,7 +9306,7 @@
         <v>7.6264907204854987E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>201</v>
       </c>
@@ -9355,7 +9356,7 @@
         <v>7.6985985651091035E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>200</v>
       </c>
@@ -9405,7 +9406,7 @@
         <v>7.9409018143009602E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>199</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>7.8426119416313916E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>198</v>
       </c>
@@ -9505,7 +9506,7 @@
         <v>7.6960509077297401E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>197</v>
       </c>
@@ -9555,7 +9556,7 @@
         <v>7.7764565992865631E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>196</v>
       </c>
@@ -9605,7 +9606,7 @@
         <v>8.6876390212901181E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>195</v>
       </c>
@@ -9655,7 +9656,7 @@
         <v>7.9463140591412421E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>194</v>
       </c>
@@ -9705,7 +9706,7 @@
         <v>7.8242611520481731E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>193</v>
       </c>
@@ -9755,7 +9756,7 @@
         <v>7.86247234824341E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>192</v>
       </c>
@@ -9805,7 +9806,7 @@
         <v>8.1036834924965898E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>191</v>
       </c>
@@ -9855,7 +9856,7 @@
         <v>7.7535727062190501E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>190</v>
       </c>
@@ -9905,7 +9906,7 @@
         <v>7.8847027678447951E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>189</v>
       </c>
@@ -9955,7 +9956,7 @@
         <v>7.962854477207143E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>188</v>
       </c>
@@ -10005,7 +10006,7 @@
         <v>7.8374628344895933E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>187</v>
       </c>
@@ -10055,7 +10056,7 @@
         <v>8.019005543283457E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>186</v>
       </c>
@@ -10105,7 +10106,7 @@
         <v>8.1247886371322284E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>185</v>
       </c>
@@ -10155,7 +10156,7 @@
         <v>8.6690765691751562E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>184</v>
       </c>
@@ -10205,7 +10206,7 @@
         <v>8.4999547634126482E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>183</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>8.0257365391127669E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>182</v>
       </c>
@@ -10305,7 +10306,7 @@
         <v>8.4161379145217291E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>181</v>
       </c>
@@ -10355,7 +10356,7 @@
         <v>8.5486340957367984E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>180</v>
       </c>
@@ -10405,7 +10406,7 @@
         <v>8.4206823777699613E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>179</v>
       </c>
@@ -10455,7 +10456,7 @@
         <v>8.0847054600924229E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -10505,7 +10506,7 @@
         <v>8.5522980736735379E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>177</v>
       </c>
@@ -10555,7 +10556,7 @@
         <v>8.4571612873499666E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>176</v>
       </c>
@@ -10605,7 +10606,7 @@
         <v>8.1390459281409144E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>175</v>
       </c>
@@ -10655,7 +10656,7 @@
         <v>8.35138234169958E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>174</v>
       </c>
@@ -10705,7 +10706,7 @@
         <v>8.361852339356228E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>173</v>
       </c>
@@ -10755,7 +10756,7 @@
         <v>8.4597360956961395E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>172</v>
       </c>
@@ -10805,7 +10806,7 @@
         <v>8.2498401193775314E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>171</v>
       </c>
@@ -10855,7 +10856,7 @@
         <v>8.0590753794922809E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>170</v>
       </c>
@@ -10905,7 +10906,7 @@
         <v>8.3553231892278479E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>169</v>
       </c>
@@ -10955,7 +10956,7 @@
         <v>8.5461589437732577E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>168</v>
       </c>
@@ -11005,7 +11006,7 @@
         <v>8.4603678196497195E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>167</v>
       </c>
@@ -11055,7 +11056,7 @@
         <v>8.444623968089672E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>166</v>
       </c>
@@ -11105,7 +11106,7 @@
         <v>8.33372480856861E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>165</v>
       </c>
@@ -11155,7 +11156,7 @@
         <v>8.4654750800413445E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>164</v>
       </c>
@@ -11205,7 +11206,7 @@
         <v>8.7245779766555384E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>163</v>
       </c>
@@ -11255,7 +11256,7 @@
         <v>8.6143376144911216E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>162</v>
       </c>
@@ -11305,7 +11306,7 @@
         <v>8.5036775795262073E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>161</v>
       </c>
@@ -11355,7 +11356,7 @@
         <v>8.4609317631700612E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>160</v>
       </c>
@@ -11405,7 +11406,7 @@
         <v>8.5424358877753501E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>159</v>
       </c>
@@ -11455,7 +11456,7 @@
         <v>8.5117773019271953E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>158</v>
       </c>
@@ -11505,7 +11506,7 @@
         <v>8.953052002757142E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>157</v>
       </c>
@@ -11555,7 +11556,7 @@
         <v>8.558253438932889E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>156</v>
       </c>
@@ -11605,7 +11606,7 @@
         <v>8.5854858548585489E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>155</v>
       </c>
@@ -11655,7 +11656,7 @@
         <v>8.5020242914979755E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>154</v>
       </c>
@@ -11705,7 +11706,7 @@
         <v>8.4892779696409931E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>153</v>
       </c>
@@ -11755,7 +11756,7 @@
         <v>8.58343949044586E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>152</v>
       </c>
@@ -11805,7 +11806,7 @@
         <v>9.0093284599858159E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>151</v>
       </c>
@@ -11855,7 +11856,7 @@
         <v>9.6823168810335439E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>150</v>
       </c>
@@ -11905,7 +11906,7 @@
         <v>8.6683515280998408E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>149</v>
       </c>
@@ -11955,7 +11956,7 @@
         <v>8.9607563995809714E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>148</v>
       </c>
@@ -12005,7 +12006,7 @@
         <v>9.1780455153949128E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>147</v>
       </c>
@@ -12055,7 +12056,7 @@
         <v>8.7407636260652399E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>146</v>
       </c>
@@ -12105,7 +12106,7 @@
         <v>8.8065593683571211E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>145</v>
       </c>
@@ -12155,7 +12156,7 @@
         <v>8.9734204302286291E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>144</v>
       </c>
@@ -12205,7 +12206,7 @@
         <v>8.3344836153824917E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>143</v>
       </c>
@@ -12255,7 +12256,7 @@
         <v>8.7958782599458218E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>142</v>
       </c>
@@ -12305,7 +12306,7 @@
         <v>8.6941368864105514E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>141</v>
       </c>
@@ -12355,7 +12356,7 @@
         <v>8.9946780513480318E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>140</v>
       </c>
@@ -12405,7 +12406,7 @@
         <v>9.0288014514117249E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>139</v>
       </c>
@@ -12455,7 +12456,7 @@
         <v>9.3769745987615311E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>138</v>
       </c>
@@ -12505,7 +12506,7 @@
         <v>8.9891451831750332E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>137</v>
       </c>
@@ -12555,7 +12556,7 @@
         <v>8.7936191425722829E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>136</v>
       </c>
@@ -12605,7 +12606,7 @@
         <v>8.8594164456233415E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>135</v>
       </c>
@@ -12655,7 +12656,7 @@
         <v>9.0789398362814133E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>134</v>
       </c>
@@ -12705,7 +12706,7 @@
         <v>8.7943471220373909E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>133</v>
       </c>
@@ -12755,7 +12756,7 @@
         <v>8.4952281343966526E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>132</v>
       </c>
@@ -12805,7 +12806,7 @@
         <v>8.9451666339107727E-2</v>
       </c>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>131</v>
       </c>
@@ -12855,7 +12856,7 @@
         <v>8.7020731163620149E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>130</v>
       </c>
@@ -12905,7 +12906,7 @@
         <v>8.7424364362574142E-2</v>
       </c>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>129</v>
       </c>
@@ -12955,7 +12956,7 @@
         <v>8.6854599406528191E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>128</v>
       </c>
@@ -13005,7 +13006,7 @@
         <v>8.642512997795139E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>127</v>
       </c>
@@ -13055,7 +13056,7 @@
         <v>8.7740523101739826E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>126</v>
       </c>
@@ -13105,7 +13106,7 @@
         <v>8.9113664735443812E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>125</v>
       </c>
@@ -13155,7 +13156,7 @@
         <v>9.4856688952141388E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>124</v>
       </c>
@@ -13205,7 +13206,7 @@
         <v>8.9612321694232958E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>123</v>
       </c>
@@ -13255,7 +13256,7 @@
         <v>8.9393939393939401E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>122</v>
       </c>
@@ -13305,7 +13306,7 @@
         <v>8.9579266049854292E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>121</v>
       </c>
@@ -13355,7 +13356,7 @@
         <v>9.1778202676864248E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>120</v>
       </c>
@@ -13405,7 +13406,7 @@
         <v>8.8148023737543393E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>119</v>
       </c>
@@ -13455,7 +13456,7 @@
         <v>9.2238145618928541E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>118</v>
       </c>
@@ -13505,7 +13506,7 @@
         <v>9.0230495346367665E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>117</v>
       </c>
@@ -13555,7 +13556,7 @@
         <v>9.0734121528732475E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:16">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>116</v>
       </c>
@@ -13605,7 +13606,7 @@
         <v>9.2319912018085176E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:16">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>115</v>
       </c>
@@ -13655,7 +13656,7 @@
         <v>9.2701342281879193E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:16">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>114</v>
       </c>
@@ -13705,7 +13706,7 @@
         <v>9.3892747637819907E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:16">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>113</v>
       </c>
@@ -13755,7 +13756,7 @@
         <v>9.0420241203531024E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:16">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>112</v>
       </c>
@@ -13805,7 +13806,7 @@
         <v>9.4982385333652566E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:16">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>111</v>
       </c>
@@ -13855,7 +13856,7 @@
         <v>9.5922831426829711E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:16">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>110</v>
       </c>
@@ -13905,7 +13906,7 @@
         <v>9.8912409510412733E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:16">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>109</v>
       </c>
@@ -13955,7 +13956,7 @@
         <v>9.1738142861985963E-2</v>
       </c>
     </row>
-    <row r="249" spans="1:16">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>108</v>
       </c>
@@ -14005,7 +14006,7 @@
         <v>9.1406881961296746E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:16">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>107</v>
       </c>
@@ -14055,7 +14056,7 @@
         <v>9.0301103646833011E-2</v>
       </c>
     </row>
-    <row r="251" spans="1:16">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>106</v>
       </c>
@@ -14105,7 +14106,7 @@
         <v>0.1106971508215176</v>
       </c>
     </row>
-    <row r="252" spans="1:16">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>105</v>
       </c>
@@ -14155,7 +14156,7 @@
         <v>9.1956430666108091E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:16">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>104</v>
       </c>
@@ -14205,7 +14206,7 @@
         <v>9.1776931907437617E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:16">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>103</v>
       </c>
@@ -14255,7 +14256,7 @@
         <v>9.7860199714693299E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:16">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>102</v>
       </c>
@@ -14305,7 +14306,7 @@
         <v>9.0897464590593724E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:16">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>101</v>
       </c>
@@ -14355,7 +14356,7 @@
         <v>9.0693019764823621E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:16">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>100</v>
       </c>
@@ -14405,7 +14406,7 @@
         <v>9.0523871716731971E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:16">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>99</v>
       </c>
@@ -14455,7 +14456,7 @@
         <v>9.1815036973563108E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:16">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>98</v>
       </c>
@@ -14505,7 +14506,7 @@
         <v>9.3876803856362698E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:16">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>97</v>
       </c>
@@ -14555,7 +14556,7 @@
         <v>9.232944747189073E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:16">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>96</v>
       </c>
@@ -14605,7 +14606,7 @@
         <v>9.0960701444521536E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:16">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>95</v>
       </c>
@@ -14655,7 +14656,7 @@
         <v>9.320639018880103E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:16">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>94</v>
       </c>
@@ -14705,7 +14706,7 @@
         <v>9.5901770052623181E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:16">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>93</v>
       </c>
@@ -14755,7 +14756,7 @@
         <v>9.2824096859927152E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:16">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>92</v>
       </c>
@@ -14805,7 +14806,7 @@
         <v>9.1567113986484316E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:16">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>91</v>
       </c>
@@ -14855,7 +14856,7 @@
         <v>9.5596057017232824E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:16">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>90</v>
       </c>
@@ -14905,7 +14906,7 @@
         <v>9.2229460249933531E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:16">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>89</v>
       </c>
@@ -14955,7 +14956,7 @@
         <v>9.1953666997026756E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:16">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>88</v>
       </c>
@@ -15005,7 +15006,7 @@
         <v>9.5583182357718496E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:16">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>87</v>
       </c>
@@ -15055,7 +15056,7 @@
         <v>9.3260061419104576E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:16">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>86</v>
       </c>
@@ -15105,7 +15106,7 @@
         <v>9.184551995572228E-2</v>
       </c>
     </row>
-    <row r="272" spans="1:16">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>85</v>
       </c>
@@ -15155,7 +15156,7 @@
         <v>9.7843312891890036E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:16">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>84</v>
       </c>
@@ -15205,7 +15206,7 @@
         <v>9.8197361085300125E-2</v>
       </c>
     </row>
-    <row r="274" spans="1:16">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>83</v>
       </c>
@@ -15255,7 +15256,7 @@
         <v>9.3917206420726554E-2</v>
       </c>
     </row>
-    <row r="275" spans="1:16">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>82</v>
       </c>
@@ -15305,7 +15306,7 @@
         <v>9.8742465957288486E-2</v>
       </c>
     </row>
-    <row r="276" spans="1:16">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>81</v>
       </c>
@@ -15355,7 +15356,7 @@
         <v>9.6307961504811898E-2</v>
       </c>
     </row>
-    <row r="277" spans="1:16">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>80</v>
       </c>
@@ -15405,7 +15406,7 @@
         <v>0.10109430208226131</v>
       </c>
     </row>
-    <row r="278" spans="1:16">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>79</v>
       </c>
@@ -15455,7 +15456,7 @@
         <v>9.8429973894179498E-2</v>
       </c>
     </row>
-    <row r="279" spans="1:16">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>78</v>
       </c>
@@ -15505,7 +15506,7 @@
         <v>9.5205147720196504E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:16">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>77</v>
       </c>
@@ -15555,7 +15556,7 @@
         <v>0.1027201263033253</v>
       </c>
     </row>
-    <row r="281" spans="1:16">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>76</v>
       </c>
@@ -15605,7 +15606,7 @@
         <v>9.3699727502544405E-2</v>
       </c>
     </row>
-    <row r="282" spans="1:16">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>75</v>
       </c>
@@ -15655,7 +15656,7 @@
         <v>9.482234801240845E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:16">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>74</v>
       </c>
@@ -15705,7 +15706,7 @@
         <v>9.8035789179365299E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:16">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>73</v>
       </c>
@@ -15755,7 +15756,7 @@
         <v>9.8651225195960743E-2</v>
       </c>
     </row>
-    <row r="285" spans="1:16">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>72</v>
       </c>
@@ -15805,7 +15806,7 @@
         <v>9.6343203089662849E-2</v>
       </c>
     </row>
-    <row r="286" spans="1:16">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>71</v>
       </c>
@@ -15855,7 +15856,7 @@
         <v>9.7566085833013239E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:16">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>70</v>
       </c>
@@ -15905,7 +15906,7 @@
         <v>9.6616696465410531E-2</v>
       </c>
     </row>
-    <row r="288" spans="1:16">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>69</v>
       </c>
@@ -15955,7 +15956,7 @@
         <v>0.1031797534068787</v>
       </c>
     </row>
-    <row r="289" spans="1:16">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>68</v>
       </c>
@@ -16005,7 +16006,7 @@
         <v>9.5623035202266213E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:16">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>67</v>
       </c>
@@ -16055,7 +16056,7 @@
         <v>9.7295617034504192E-2</v>
       </c>
     </row>
-    <row r="291" spans="1:16">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>66</v>
       </c>
@@ -16105,7 +16106,7 @@
         <v>9.6597145993413833E-2</v>
       </c>
     </row>
-    <row r="292" spans="1:16">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>65</v>
       </c>
@@ -16155,7 +16156,7 @@
         <v>9.4715491325292472E-2</v>
       </c>
     </row>
-    <row r="293" spans="1:16">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>64</v>
       </c>
@@ -16205,7 +16206,7 @@
         <v>9.4463357821178998E-2</v>
       </c>
     </row>
-    <row r="294" spans="1:16">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>63</v>
       </c>
@@ -16255,7 +16256,7 @@
         <v>0.1008109397360471</v>
       </c>
     </row>
-    <row r="295" spans="1:16">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>62</v>
       </c>
@@ -16305,7 +16306,7 @@
         <v>0.10116731517509731</v>
       </c>
     </row>
-    <row r="296" spans="1:16">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>61</v>
       </c>
@@ -16355,7 +16356,7 @@
         <v>9.7063929353158732E-2</v>
       </c>
     </row>
-    <row r="297" spans="1:16">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>60</v>
       </c>
@@ -16405,7 +16406,7 @@
         <v>0.13333575739946191</v>
       </c>
     </row>
-    <row r="298" spans="1:16">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>59</v>
       </c>
@@ -16455,7 +16456,7 @@
         <v>9.541019154318757E-2</v>
       </c>
     </row>
-    <row r="299" spans="1:16">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>58</v>
       </c>
@@ -16505,7 +16506,7 @@
         <v>9.538471949651485E-2</v>
       </c>
     </row>
-    <row r="300" spans="1:16">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>57</v>
       </c>
@@ -16555,7 +16556,7 @@
         <v>9.3852908891328204E-2</v>
       </c>
     </row>
-    <row r="301" spans="1:16">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>56</v>
       </c>
@@ -16605,7 +16606,7 @@
         <v>9.2492351141445051E-2</v>
       </c>
     </row>
-    <row r="302" spans="1:16">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>55</v>
       </c>
@@ -16655,7 +16656,7 @@
         <v>9.6980816273979656E-2</v>
       </c>
     </row>
-    <row r="303" spans="1:16">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>54</v>
       </c>
@@ -16705,7 +16706,7 @@
         <v>9.3462599632127524E-2</v>
       </c>
     </row>
-    <row r="304" spans="1:16">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>53</v>
       </c>
@@ -16755,7 +16756,7 @@
         <v>9.3007018704295744E-2</v>
       </c>
     </row>
-    <row r="305" spans="1:16">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>52</v>
       </c>
@@ -16805,7 +16806,7 @@
         <v>9.2395804581838256E-2</v>
       </c>
     </row>
-    <row r="306" spans="1:16">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>51</v>
       </c>
@@ -16855,7 +16856,7 @@
         <v>9.3748862271088945E-2</v>
       </c>
     </row>
-    <row r="307" spans="1:16">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>50</v>
       </c>
@@ -16905,7 +16906,7 @@
         <v>9.3794483130073478E-2</v>
       </c>
     </row>
-    <row r="308" spans="1:16">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>49</v>
       </c>
@@ -16955,7 +16956,7 @@
         <v>9.5539334955393351E-2</v>
       </c>
     </row>
-    <row r="309" spans="1:16">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>48</v>
       </c>
@@ -17005,7 +17006,7 @@
         <v>0.10025911899541561</v>
       </c>
     </row>
-    <row r="310" spans="1:16">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>47</v>
       </c>
@@ -17055,7 +17056,7 @@
         <v>9.2968043412722343E-2</v>
       </c>
     </row>
-    <row r="311" spans="1:16">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>46</v>
       </c>
@@ -17105,7 +17106,7 @@
         <v>9.6451319381255687E-2</v>
       </c>
     </row>
-    <row r="312" spans="1:16">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>45</v>
       </c>
@@ -17155,7 +17156,7 @@
         <v>9.9350954019393187E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:16">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>44</v>
       </c>
@@ -17205,7 +17206,7 @@
         <v>9.2117240123793923E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:16">
+    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>43</v>
       </c>
@@ -17255,7 +17256,7 @@
         <v>9.9253629142700625E-2</v>
       </c>
     </row>
-    <row r="315" spans="1:16">
+    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>42</v>
       </c>
@@ -17305,7 +17306,7 @@
         <v>9.6973615095559421E-2</v>
       </c>
     </row>
-    <row r="316" spans="1:16">
+    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>41</v>
       </c>
@@ -17355,7 +17356,7 @@
         <v>9.5874514825337126E-2</v>
       </c>
     </row>
-    <row r="317" spans="1:16">
+    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>40</v>
       </c>
@@ -17405,7 +17406,7 @@
         <v>9.8073122529644272E-2</v>
       </c>
     </row>
-    <row r="318" spans="1:16">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>39</v>
       </c>
@@ -17455,7 +17456,7 @@
         <v>9.2357036119109226E-2</v>
       </c>
     </row>
-    <row r="319" spans="1:16">
+    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>38</v>
       </c>
@@ -17505,7 +17506,7 @@
         <v>9.1925139706709666E-2</v>
       </c>
     </row>
-    <row r="320" spans="1:16">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>37</v>
       </c>
@@ -17555,7 +17556,7 @@
         <v>9.8357697166576427E-2</v>
       </c>
     </row>
-    <row r="321" spans="1:16">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>36</v>
       </c>
@@ -17605,7 +17606,7 @@
         <v>9.625160143819482E-2</v>
       </c>
     </row>
-    <row r="322" spans="1:16">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>34</v>
       </c>
@@ -17655,7 +17656,7 @@
         <v>9.3469808775688334E-2</v>
       </c>
     </row>
-    <row r="323" spans="1:16">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>33</v>
       </c>
@@ -17705,7 +17706,7 @@
         <v>9.5351426048904078E-2</v>
       </c>
     </row>
-    <row r="324" spans="1:16">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>32</v>
       </c>
@@ -17755,7 +17756,7 @@
         <v>9.7560975609756101E-2</v>
       </c>
     </row>
-    <row r="325" spans="1:16">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>30</v>
       </c>
@@ -17805,7 +17806,7 @@
         <v>9.72246773908432E-2</v>
       </c>
     </row>
-    <row r="326" spans="1:16">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>29</v>
       </c>
@@ -17855,7 +17856,7 @@
         <v>9.5066136492737152E-2</v>
       </c>
     </row>
-    <row r="327" spans="1:16">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A327" s="1">
         <v>28</v>
       </c>
@@ -17905,7 +17906,7 @@
         <v>9.4667616135383062E-2</v>
       </c>
     </row>
-    <row r="328" spans="1:16">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A328" s="1">
         <v>27</v>
       </c>
@@ -17955,7 +17956,7 @@
         <v>9.3756109004183449E-2</v>
       </c>
     </row>
-    <row r="329" spans="1:16">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A329" s="1">
         <v>26</v>
       </c>
@@ -18005,7 +18006,7 @@
         <v>9.5020083790437526E-2</v>
       </c>
     </row>
-    <row r="330" spans="1:16">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A330" s="1">
         <v>25</v>
       </c>
@@ -18055,7 +18056,7 @@
         <v>9.6175932621549193E-2</v>
       </c>
     </row>
-    <row r="331" spans="1:16">
+    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A331" s="1">
         <v>24</v>
       </c>
@@ -18105,7 +18106,7 @@
         <v>9.5907466163299732E-2</v>
       </c>
     </row>
-    <row r="332" spans="1:16">
+    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A332" s="1">
         <v>23</v>
       </c>
@@ -18155,7 +18156,7 @@
         <v>8.7881503844520967E-2</v>
       </c>
     </row>
-    <row r="333" spans="1:16">
+    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A333" s="1">
         <v>22</v>
       </c>
@@ -18205,7 +18206,7 @@
         <v>9.1582064297800345E-2</v>
       </c>
     </row>
-    <row r="334" spans="1:16">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A334" s="1">
         <v>21</v>
       </c>
@@ -18255,7 +18256,7 @@
         <v>9.6469253674906649E-2</v>
       </c>
     </row>
-    <row r="335" spans="1:16">
+    <row r="335" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A335" s="1">
         <v>20</v>
       </c>
@@ -18266,7 +18267,7 @@
         <v>540</v>
       </c>
       <c r="D335" t="s">
-        <v>339</v>
+        <v>367</v>
       </c>
       <c r="E335">
         <v>21947</v>
@@ -18305,7 +18306,7 @@
         <v>9.4545951610698495E-2</v>
       </c>
     </row>
-    <row r="336" spans="1:16">
+    <row r="336" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A336" s="1">
         <v>19</v>
       </c>
@@ -18316,7 +18317,7 @@
         <v>541</v>
       </c>
       <c r="D336" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E336">
         <v>22873</v>
@@ -18355,7 +18356,7 @@
         <v>9.3997289380492288E-2</v>
       </c>
     </row>
-    <row r="337" spans="1:16">
+    <row r="337" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A337" s="1">
         <v>18</v>
       </c>
@@ -18366,7 +18367,7 @@
         <v>542</v>
       </c>
       <c r="D337" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E337">
         <v>24101</v>
@@ -18405,7 +18406,7 @@
         <v>9.2278328700053938E-2</v>
       </c>
     </row>
-    <row r="338" spans="1:16">
+    <row r="338" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A338" s="1">
         <v>17</v>
       </c>
@@ -18416,7 +18417,7 @@
         <v>543</v>
       </c>
       <c r="D338" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E338">
         <v>20824</v>
@@ -18455,7 +18456,7 @@
         <v>9.8348059930849024E-2</v>
       </c>
     </row>
-    <row r="339" spans="1:16">
+    <row r="339" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A339" s="1">
         <v>16</v>
       </c>
@@ -18466,7 +18467,7 @@
         <v>544</v>
       </c>
       <c r="D339" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E339">
         <v>22176</v>
@@ -18505,7 +18506,7 @@
         <v>9.5914502164502161E-2</v>
       </c>
     </row>
-    <row r="340" spans="1:16">
+    <row r="340" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A340" s="1">
         <v>14</v>
       </c>
@@ -18516,7 +18517,7 @@
         <v>546</v>
       </c>
       <c r="D340" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E340">
         <v>22336</v>
@@ -18555,7 +18556,7 @@
         <v>9.3481375358166183E-2</v>
       </c>
     </row>
-    <row r="341" spans="1:16">
+    <row r="341" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A341" s="1">
         <v>13</v>
       </c>
@@ -18566,7 +18567,7 @@
         <v>547</v>
       </c>
       <c r="D341" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E341">
         <v>22166</v>
@@ -18605,7 +18606,7 @@
         <v>9.5100604529459537E-2</v>
       </c>
     </row>
-    <row r="342" spans="1:16">
+    <row r="342" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A342" s="1">
         <v>12</v>
       </c>
@@ -18616,7 +18617,7 @@
         <v>548</v>
       </c>
       <c r="D342" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E342">
         <v>26010</v>
@@ -18655,7 +18656,7 @@
         <v>9.311803152633602E-2</v>
       </c>
     </row>
-    <row r="343" spans="1:16">
+    <row r="343" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A343" s="1">
         <v>11</v>
       </c>
@@ -18666,7 +18667,7 @@
         <v>549</v>
       </c>
       <c r="D343" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E343">
         <v>24137</v>
@@ -18705,7 +18706,7 @@
         <v>9.3673613125077687E-2</v>
       </c>
     </row>
-    <row r="344" spans="1:16">
+    <row r="344" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A344" s="1">
         <v>10</v>
       </c>
@@ -18716,7 +18717,7 @@
         <v>550</v>
       </c>
       <c r="D344" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E344">
         <v>22180</v>
@@ -18755,7 +18756,7 @@
         <v>9.1794409377817854E-2</v>
       </c>
     </row>
-    <row r="345" spans="1:16">
+    <row r="345" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A345" s="1">
         <v>9</v>
       </c>
@@ -18766,7 +18767,7 @@
         <v>551</v>
       </c>
       <c r="D345" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E345">
         <v>20490</v>
@@ -18805,7 +18806,7 @@
         <v>9.9267935578330899E-2</v>
       </c>
     </row>
-    <row r="346" spans="1:16">
+    <row r="346" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A346" s="1">
         <v>8</v>
       </c>
@@ -18816,7 +18817,7 @@
         <v>552</v>
       </c>
       <c r="D346" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E346">
         <v>21937</v>
@@ -18855,7 +18856,7 @@
         <v>9.6275698591420891E-2</v>
       </c>
     </row>
-    <row r="347" spans="1:16">
+    <row r="347" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A347" s="1">
         <v>7</v>
       </c>
@@ -18866,7 +18867,7 @@
         <v>553</v>
       </c>
       <c r="D347" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E347">
         <v>20281</v>
@@ -18905,7 +18906,7 @@
         <v>9.4226122972240034E-2</v>
       </c>
     </row>
-    <row r="348" spans="1:16">
+    <row r="348" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A348" s="1">
         <v>6</v>
       </c>
@@ -18916,7 +18917,7 @@
         <v>554</v>
       </c>
       <c r="D348" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E348">
         <v>15554</v>
@@ -18955,7 +18956,7 @@
         <v>0.10042432814710039</v>
       </c>
     </row>
-    <row r="349" spans="1:16">
+    <row r="349" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A349" s="1">
         <v>5</v>
       </c>
@@ -18966,7 +18967,7 @@
         <v>555</v>
       </c>
       <c r="D349" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E349">
         <v>20011</v>
@@ -19005,7 +19006,7 @@
         <v>0.1020938483833891</v>
       </c>
     </row>
-    <row r="350" spans="1:16">
+    <row r="350" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A350" s="1">
         <v>4</v>
       </c>
@@ -19016,7 +19017,7 @@
         <v>556</v>
       </c>
       <c r="D350" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E350">
         <v>20879</v>
@@ -19055,7 +19056,7 @@
         <v>9.636476842760669E-2</v>
       </c>
     </row>
-    <row r="351" spans="1:16">
+    <row r="351" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A351" s="1">
         <v>3</v>
       </c>
@@ -19066,7 +19067,7 @@
         <v>557</v>
       </c>
       <c r="D351" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E351">
         <v>20160</v>
@@ -19105,7 +19106,7 @@
         <v>9.6081349206349212E-2</v>
       </c>
     </row>
-    <row r="352" spans="1:16">
+    <row r="352" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A352" s="1">
         <v>2</v>
       </c>
@@ -19116,7 +19117,7 @@
         <v>558</v>
       </c>
       <c r="D352" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E352">
         <v>20001</v>
@@ -19155,7 +19156,7 @@
         <v>9.5945202739863011E-2</v>
       </c>
     </row>
-    <row r="353" spans="1:16">
+    <row r="353" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A353" s="1">
         <v>1</v>
       </c>
@@ -19166,7 +19167,7 @@
         <v>559</v>
       </c>
       <c r="D353" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E353">
         <v>21204</v>
@@ -19205,7 +19206,7 @@
         <v>9.3048481418600268E-2</v>
       </c>
     </row>
-    <row r="354" spans="1:16">
+    <row r="354" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A354" s="1">
         <v>0</v>
       </c>
@@ -19216,7 +19217,7 @@
         <v>560</v>
       </c>
       <c r="D354" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E354">
         <v>20380</v>

</xml_diff>